<commit_message>
Screenshot etc for Marty
</commit_message>
<xml_diff>
--- a/Asset List.xlsx
+++ b/Asset List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler Hales\Documents\Ty-Guy\Fall 2019\DGM 2221\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Ty-Guy\UVU\Fall 2019\DGM 2221\Git Repo\DGM2221\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8B1FBF-946F-4876-A837-F480B8A2646F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159A520-0D38-4FD9-AE13-BBAE632C51CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{78917EDD-88E5-43C4-92C3-F10BE42951DC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{78917EDD-88E5-43C4-92C3-F10BE42951DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Project Scene Asset List:</t>
   </si>
@@ -108,14 +108,29 @@
     <t>Middle Ground Platforms (Moving)</t>
   </si>
   <si>
-    <t>Textures:</t>
+    <t>Whitebox:</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>UV:</t>
+  </si>
+  <si>
+    <t>Texture:</t>
+  </si>
+  <si>
+    <t>VFX:</t>
+  </si>
+  <si>
+    <t>Animation:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,16 +138,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,14 +192,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,145 +536,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32BCBA8-CD9B-4806-AF63-CD9DB5BC2C96}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>